<commit_message>
added required_roles custom function test, closes #162
</commit_message>
<xml_diff>
--- a/tests/e2e_custom_functions.xlsx
+++ b/tests/e2e_custom_functions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/dev/xlwings-server/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088B0606-4991-C94C-B8B3-587DDDD8F398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A564224-9359-414F-B13D-0CBD833E7293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="900" yWindow="780" windowWidth="33300" windowHeight="21360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
       </extLst>
     </bk>
   </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="8">
+  <futureMetadata name="XLRICHVALUE" count="9">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -104,13 +104,20 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="8"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="8">
+  <valueMetadata count="9">
     <bk>
       <rc t="2" v="0"/>
     </bk>
@@ -135,12 +142,15 @@
     <bk>
       <rc t="2" v="7"/>
     </bk>
+    <bk>
+      <rc t="2" v="8"/>
+    </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="143">
   <si>
     <t>epected</t>
   </si>
@@ -566,6 +576,9 @@
   </si>
   <si>
     <t>varargs_with_object_handles</t>
+  </si>
+  <si>
+    <t>required_roles</t>
   </si>
 </sst>
 </file>
@@ -826,7 +839,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="8">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="9">
   <rv s="0">
     <fb>25568</fb>
     <v>0</v>
@@ -863,11 +876,14 @@
     <v>(5, 3)</v>
     <v>DataFrame</v>
   </rv>
+  <rv s="2">
+    <v>16</v>
+  </rv>
 </rvData>
 </file>
 
 <file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="3">
   <s t="_formattednumber">
     <k n="_Format" t="spb"/>
   </s>
@@ -878,6 +894,9 @@
     <k n="Index" t="s"/>
     <k n="Shape" t="s"/>
     <k n="Type" t="s"/>
+  </s>
+  <s t="_error">
+    <k n="errorType" t="i"/>
   </s>
 </rvStructures>
 </file>
@@ -1474,6 +1493,7 @@
         <we:customFunctionIds>_xldudf_XLWINGS_DEV_READ_VERTICAL_LIST</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGS_DEV_READ_VERTICAL_NPARRAY</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGS_DEV_READ_WORKBOOK_CALLER</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGS_DEV_REQUIRED_ROLES</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGS_DEV_RETURN_PD_NAT</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGS_DEV_SQL</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGS_DEV_STANDARD_NORMAL</we:customFunctionIds>
@@ -1496,6 +1516,7 @@
         <we:customFunctionIds>_xldudf_XLWINGS_DEV_TYPE_HINTS_RET_DF_ANNOTATED</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGS_DEV_TYPE_HINTS_RET_DF_DECORATOR_OVERRIDE</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGS_DEV_VARARGS_ARG_DECORATOR</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGS_DEV_VARARGS_WITH_OBJECT_HANDLES</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGS_DEV_VARIABLE_ARGS</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGS_DEV_VIEW</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGS_DEV_VOLATILE</we:customFunctionIds>
@@ -1544,10 +1565,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:P407"/>
+  <dimension ref="A1:P409"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8141,6 +8162,23 @@
       <c r="F407" t="e" cm="1" vm="8">
         <f t="array" ref="F407">_xldudf_XLWINGS_DEV_GET_DF()</f>
         <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="409" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A409" t="b">
+        <f>G409</f>
+        <v>1</v>
+      </c>
+      <c r="B409" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="F409" t="e" cm="1" vm="9">
+        <f t="array" ref="F409">_xldudf_XLWINGS_DEV_REQUIRED_ROLES()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G409" s="2" t="b">
+        <f>ISERROR(F409)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>